<commit_message>
update planilha de atividades 15/05
</commit_message>
<xml_diff>
--- a/Planílha_de_Atividades.xlsx
+++ b/Planílha_de_Atividades.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.oliveira\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.oliveira\Documents\LucasAraujo_Interalpha\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Data</t>
   </si>
@@ -41,7 +41,10 @@
     <t>Folga</t>
   </si>
   <si>
-    <t>Durante a manhã deletei os itens do menu do sistema das paginas que foram deletada.</t>
+    <t>Deletei os itens do menu do sistema das páginas que foram deletada e terminei de deletar as tabelas, views e classes que ainda faltavam.</t>
+  </si>
+  <si>
+    <t>Cadastrei no BD novos itens no Menu de Páginas que ainda serão implementadas.</t>
   </si>
 </sst>
 </file>
@@ -404,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,12 +459,20 @@
         <v>43233</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3">
         <v>43234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>43235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>